<commit_message>
Completed 1952 portion of replication
</commit_message>
<xml_diff>
--- a/RawData/IntlData1952.xlsx
+++ b/RawData/IntlData1952.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bpaye\Dropbox\Research\JEFBreaks\pt-jemf-2006\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF50A1DB-F0D4-4ED3-BAFE-3CC8E906F74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FAECDE-F802-42CB-B5DF-8D67EFAEB736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2013,13 +2013,13 @@
     <t>lagUK_DY</t>
   </si>
   <si>
-    <t>lagUSTerm</t>
-  </si>
-  <si>
-    <t>lagUS_Def</t>
-  </si>
-  <si>
     <t>UKeret</t>
+  </si>
+  <si>
+    <t>lagUS_DEF</t>
+  </si>
+  <si>
+    <t>lagUS_Term</t>
   </si>
 </sst>
 </file>
@@ -2918,7 +2918,7 @@
   <dimension ref="A1:Q620"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2952,7 +2952,7 @@
         <v>627</v>
       </c>
       <c r="J1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="K1" t="s">
         <v>628</v>
@@ -2973,7 +2973,7 @@
         <v>657</v>
       </c>
       <c r="Q1" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.45">

</xml_diff>